<commit_message>
Added Credit Limit Filter #1.0.8
-Tested safe to merge
-Updated Account selection and fetcher logic
</commit_message>
<xml_diff>
--- a/src/main/resources/credentials/accounts.xlsx
+++ b/src/main/resources/credentials/accounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srivi/IdeaProjects/ProfitCalculator/src/main/resources/credentials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCD7B2D-CB55-374E-8A0E-7FF05266B8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E418C5-944C-B34F-A189-BA0A809844FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{27BFE91B-246E-2E4A-9862-F3D86B54AF0C}"/>
+    <workbookView xWindow="20040" yWindow="500" windowWidth="18360" windowHeight="19900" xr2:uid="{27BFE91B-246E-2E4A-9862-F3D86B54AF0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>Password</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t>T047W271</t>
+  </si>
+  <si>
+    <t>Credit Limit</t>
+  </si>
+  <si>
+    <t>Account Set 6</t>
+  </si>
+  <si>
+    <t>T0XXXXX</t>
   </si>
 </sst>
 </file>
@@ -511,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3D7D20-2599-0540-AFA8-8C3AE1A99BF6}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,7 +534,7 @@
     <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -550,8 +559,11 @@
       <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -576,8 +588,11 @@
       <c r="H2" t="s">
         <v>7</v>
       </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -602,8 +617,11 @@
       <c r="H3" t="s">
         <v>10</v>
       </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -628,8 +646,11 @@
       <c r="H4" t="s">
         <v>7</v>
       </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -654,8 +675,11 @@
       <c r="H5" t="s">
         <v>10</v>
       </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -679,6 +703,38 @@
       </c>
       <c r="H6" t="s">
         <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Excel Util to handle Dynamic Account set Build #1.1.3 - Added Loading UI elements for Android and iOS Utility - Updated Selenium function to stop executing when one test fails - Added Learn More options to know more about features - Tested Safe To Merge
</commit_message>
<xml_diff>
--- a/src/main/resources/credentials/accounts.xlsx
+++ b/src/main/resources/credentials/accounts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srivi/IdeaProjects/ProfitCalculator/src/main/resources/credentials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srivi/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E418C5-944C-B34F-A189-BA0A809844FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32B0D3A-9E84-FD41-A0CC-DB39C3854249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20040" yWindow="500" windowWidth="18360" windowHeight="19900" xr2:uid="{27BFE91B-246E-2E4A-9862-F3D86B54AF0C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>Password</t>
   </si>
@@ -110,19 +110,7 @@
     <t>Auto@467</t>
   </si>
   <si>
-    <t>Account Set 5</t>
-  </si>
-  <si>
-    <t>T047W271</t>
-  </si>
-  <si>
     <t>Credit Limit</t>
-  </si>
-  <si>
-    <t>Account Set 6</t>
-  </si>
-  <si>
-    <t>T0XXXXX</t>
   </si>
 </sst>
 </file>
@@ -520,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3D7D20-2599-0540-AFA8-8C3AE1A99BF6}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,7 +548,7 @@
         <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -677,64 +665,6 @@
       </c>
       <c r="I5" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>